<commit_message>
implemented excel util from https://www.toolsqa.com/selenium-webdriver/testng-data-provider-excel/
</commit_message>
<xml_diff>
--- a/src/test/java/resources/data-provider.xlsx
+++ b/src/test/java/resources/data-provider.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\dataprovider\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064021A5-4F1C-4E37-AF6E-ADF553BB5D59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61B08B9-40A3-46FC-B68C-197F494ACD86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{13A558D3-74B5-4017-8981-F25E3D8BC0C0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{13A558D3-74B5-4017-8981-F25E3D8BC0C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>NAME</t>
   </si>
@@ -76,13 +77,37 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>User 1</t>
+  </si>
+  <si>
+    <t>User 2</t>
+  </si>
+  <si>
+    <t>testuser1</t>
+  </si>
+  <si>
+    <t>testuser2</t>
+  </si>
+  <si>
+    <t>Test@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +119,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,14 +149,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B540A8A-6443-41CB-BAD5-6C91214CDB11}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -553,4 +597,60 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918C8C99-0912-4FB0-8A29-E35407F19041}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="16.33203125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2D6E844A-09F4-43E6-836E-15645B9EBCBE}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{053D4EA9-1CB2-4C52-A207-BD1B32423A3F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>